<commit_message>
GetColumnLO + GetRowLO + ResizeLO
</commit_message>
<xml_diff>
--- a/tests/MiscTables/MiscTablesTests.xlsx
+++ b/tests/MiscTables/MiscTablesTests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aa\MiscVBAFunctions\tests\MiscTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA\MiscVBAFunctions\tests\MiscTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BCC6DF-4848-4648-900C-72F9D7F16B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C39F04-458F-4E7A-9CA4-A99470F5972C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Column1</t>
   </si>
@@ -44,6 +44,15 @@
   </si>
   <si>
     <t>SheetScopedNamedRange1</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
   </si>
 </sst>
 </file>
@@ -108,10 +117,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{882CA171-DD10-480E-80F9-30BFF0C0D9DA}" name="Table1" displayName="Table1" ref="C5:C6" insertRow="1" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{882CA171-DD10-480E-80F9-30BFF0C0D9DA}" name="Table1" displayName="Table1" ref="C5:C6" totalsRowShown="0">
   <autoFilter ref="C5:C6" xr:uid="{882CA171-DD10-480E-80F9-30BFF0C0D9DA}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{64374189-AFB6-41C1-BF33-897B4B7BA8C8}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FBDFD974-737D-4A86-BFD2-0E32834102BE}" name="Table2" displayName="Table2" ref="L4:N7" totalsRowShown="0">
+  <autoFilter ref="L4:N7" xr:uid="{FBDFD974-737D-4A86-BFD2-0E32834102BE}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{1119759B-6910-411E-868E-8D6194477B6C}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{3472BDC4-61F5-4A89-B7F5-F0FF0FF57359}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{E6145BA2-443D-4513-A14E-5EFEB9D132E7}" name="Column3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -381,18 +402,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="C3:I6"/>
+  <dimension ref="C3:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="12" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
@@ -403,7 +425,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -413,20 +446,53 @@
       <c r="I5" t="s">
         <v>0</v>
       </c>
+      <c r="L5">
+        <v>11</v>
+      </c>
+      <c r="M5">
+        <v>12</v>
+      </c>
+      <c r="N5">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
       <c r="F6" t="s">
         <v>3</v>
       </c>
       <c r="I6" t="s">
         <v>3</v>
+      </c>
+      <c r="L6">
+        <v>21</v>
+      </c>
+      <c r="M6">
+        <v>22</v>
+      </c>
+      <c r="N6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>31</v>
+      </c>
+      <c r="M7">
+        <v>32</v>
+      </c>
+      <c r="N7">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bugfix `=` autocorrect in copytable
</commit_message>
<xml_diff>
--- a/tests/MiscTables/MiscTablesTests.xlsx
+++ b/tests/MiscTables/MiscTablesTests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA\MiscVBAFunctions\tests\MiscTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aa\MiscVBAFunctions\tests\MiscTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716EE3D0-0B7E-4F3B-B31B-A76FFCECAA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB46EFE-B6B0-4DE7-A949-CCD8E0679E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="2670" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16308" yWindow="-16308" windowWidth="38616" windowHeight="15696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,28 @@
     <definedName name="NamedRange1">Sheet1!$F$5:$F$6</definedName>
     <definedName name="SheetScopedNamedRange1" localSheetId="0">Sheet1!$I$5:$I$6</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Column1</t>
   </si>
@@ -50,6 +61,12 @@
   </si>
   <si>
     <t>Column3</t>
+  </si>
+  <si>
+    <t>=[foo]</t>
+  </si>
+  <si>
+    <t>Hello</t>
   </si>
 </sst>
 </file>
@@ -96,13 +113,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,20 +449,20 @@
   <dimension ref="C3:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
     <col min="6" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
@@ -455,7 +473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.3">
       <c r="L4" s="5" t="s">
         <v>0</v>
       </c>
@@ -466,7 +484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -486,7 +504,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F6" t="s">
         <v>3</v>
       </c>
@@ -503,7 +521,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
       <c r="L7" s="5">
         <v>31</v>
       </c>
@@ -514,7 +532,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F9" s="5" t="s">
         <v>0</v>
       </c>
@@ -522,7 +540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F10">
         <v>11</v>
       </c>
@@ -530,7 +548,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F11">
         <v>21</v>
       </c>
@@ -538,7 +556,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F12">
         <v>31</v>
       </c>
@@ -546,7 +564,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
       <c r="M14" t="s">
         <v>0</v>
       </c>
@@ -554,15 +572,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="M15">
-        <v>11</v>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="M15" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="N15" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:14" x14ac:dyDescent="0.3">
       <c r="M16" s="2">
         <v>21</v>
       </c>
@@ -570,9 +588,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M17">
-        <v>31</v>
+    <row r="17" spans="13:14" x14ac:dyDescent="0.3">
+      <c r="M17" t="s">
+        <v>8</v>
       </c>
       <c r="N17" s="3">
         <v>32</v>

</xml_diff>

<commit_message>
bugfix - dont copy formats of previous row
Using LO.ListRows.Add, it copies the formatting of the previous
row. If a row above has a `=[foo]` value, it will be formatted as text
and result in error if the next row's item should not be formatted
as text. For example R21.00 ended up being
'$21.00' as string instead of the value 21
</commit_message>
<xml_diff>
--- a/tests/MiscTables/MiscTablesTests.xlsx
+++ b/tests/MiscTables/MiscTablesTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aa\MiscVBAFunctions\tests\MiscTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB46EFE-B6B0-4DE7-A949-CCD8E0679E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12672B56-992C-4AEC-A529-E53E6E5051F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16308" yWindow="-16308" windowWidth="38616" windowHeight="15696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,8 +39,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Column1</t>
   </si>
@@ -67,6 +89,9 @@
   </si>
   <si>
     <t>Hello</t>
+  </si>
+  <si>
+    <t>=foo</t>
   </si>
 </sst>
 </file>
@@ -149,11 +174,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E6030458-C416-437F-B373-5484DD0DB1B9}" name="TableForCopy" displayName="TableForCopy" ref="M14:N17" totalsRowShown="0">
-  <autoFilter ref="M14:N17" xr:uid="{E6030458-C416-437F-B373-5484DD0DB1B9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E6030458-C416-437F-B373-5484DD0DB1B9}" name="TableForCopy" displayName="TableForCopy" ref="M14:N19">
+  <autoFilter ref="M14:N19" xr:uid="{E6030458-C416-437F-B373-5484DD0DB1B9}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{37F285BA-1041-4652-AAFA-37EBFEDC46F1}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{D22B3F94-5A2B-4375-8EE3-FEE91D070AC9}" name="Column2"/>
+    <tableColumn id="1" xr3:uid="{37F285BA-1041-4652-AAFA-37EBFEDC46F1}" name="Column1" totalsRowFunction="custom">
+      <totalsRowFormula array="1">NameError</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{D22B3F94-5A2B-4375-8EE3-FEE91D070AC9}" name="Column2" totalsRowFunction="custom">
+      <totalsRowFormula>NA()</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -446,10 +475,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="C3:N17"/>
+  <dimension ref="C3:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,6 +625,24 @@
         <v>32</v>
       </c>
     </row>
+    <row r="18" spans="13:14" x14ac:dyDescent="0.3">
+      <c r="M18" s="5" t="e" cm="1">
+        <f t="array" ref="M18">NameError</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N18" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="13:14" x14ac:dyDescent="0.3">
+      <c r="M19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N19">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed array indexing in RangeToArray
</commit_message>
<xml_diff>
--- a/tests/MiscTables/MiscTablesTests.xlsx
+++ b/tests/MiscTables/MiscTablesTests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AA\MiscVBAFunctions\tests\MiscTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059A8729-9079-4EBB-836A-F1F18685C16E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2495154D-076D-47ED-B484-D42BF4658027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>Column1</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>=foo</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>aaa</t>
   </si>
 </sst>
 </file>
@@ -228,6 +237,16 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{04793A33-8E3C-4B1D-91D1-A71EE4265266}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{55015F3C-305A-4C88-AB92-50C4A528FF81}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{066B24FC-0ED0-4703-9EAE-73B5DB8C6230}" name="Table7" displayName="Table7" ref="G3:G4" totalsRowShown="0">
+  <autoFilter ref="G3:G4" xr:uid="{066B24FC-0ED0-4703-9EAE-73B5DB8C6230}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{EB0F03F3-7D59-4C12-9076-FF9AFB7CDDA6}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -680,19 +699,21 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CD61AF-9700-4552-A9AB-E92AAA6F6855}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A3:E3"/>
+  <dimension ref="A3:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E5"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="10.5546875" customWidth="1"/>
     <col min="4" max="5" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -705,12 +726,35 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>